<commit_message>
Console UI decoupling. Reordered Classes.
</commit_message>
<xml_diff>
--- a/Отборна патерни.xlsx
+++ b/Отборна патерни.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Behavioral</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Memento???</t>
   </si>
   <si>
-    <t>Prototype</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -104,13 +101,42 @@
   </si>
   <si>
     <t>Използване на отделни класове за различните команди, които потребителя подава</t>
+  </si>
+  <si>
+    <t>Abstract Factory</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">creating commands via </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ICommandFactory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>  interface</t>
+    </r>
+  </si>
+  <si>
+    <t>Lazy initialization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +182,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -195,9 +233,6 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -218,6 +253,9 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,176 +580,180 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>